<commit_message>
Changed requests to AsyncClient in celery task
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -278,7 +278,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
@@ -406,7 +406,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>168.25</v>
+        <v>168.21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>